<commit_message>
grado 11 - guion 08 - Esqueleto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion08/esqueletoGuion - CS_11_08_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion08/esqueletoGuion - CS_11_08_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="78">
   <si>
     <t>FICHA</t>
   </si>
@@ -139,42 +139,6 @@
     <t>Ciencias Sociales</t>
   </si>
   <si>
-    <t>Eso 4/ Ciencias Sociales/ el mundo actual/ Las potencias emergentes: Brasil, Rusia, India y China</t>
-  </si>
-  <si>
-    <t>ESO 4</t>
-  </si>
-  <si>
-    <t>El mundo actual</t>
-  </si>
-  <si>
-    <t>Las potencias emergentes: Brasil, Rusia, India y China</t>
-  </si>
-  <si>
-    <t>Eso 4/ Ciencias Sociales/El mundo actual / Los conflictos recientes/</t>
-  </si>
-  <si>
-    <t>Los conflictos recientes</t>
-  </si>
-  <si>
-    <t>El mundo islámico: entre la tradición y el cambio</t>
-  </si>
-  <si>
-    <t>Eso 4/Ciencias Sociales/El mundo actual/El mundo islámico: entre la tradición y el cambio</t>
-  </si>
-  <si>
-    <t>Este recursos requiere ajustes de imágenes</t>
-  </si>
-  <si>
-    <t>Eso 3/ Ciencias Sociales/El mundo actual: cambios y contrastes / La Primavera Árábe/</t>
-  </si>
-  <si>
-    <t>El mundo actual: cambios y contrastes</t>
-  </si>
-  <si>
-    <t>La Primavera árabe</t>
-  </si>
-  <si>
     <t>CS_11_08_CO</t>
   </si>
   <si>
@@ -265,14 +229,50 @@
     <t>Webs de referencia</t>
   </si>
   <si>
-    <t>Nuestra sociedad</t>
+    <t>Las sociedades humanas</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Profundiza: la sociedad</t>
+  </si>
+  <si>
+    <t>ESO 2</t>
+  </si>
+  <si>
+    <t>La organización del mundo actual</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Los tipos de sociedad: identifica los distintos modelos de sociedad</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Los tipos de sociedad: identifica características de cada modelo de sociedad</t>
+  </si>
+  <si>
+    <t>REC 40. Identifica características de cada modelo de sociedad</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Los tipos de sociedad/Profundiza: modelos de sociedad</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/La sociedad y la cultura/ Sociedad y cultura: la diversidad cultural en el mundo</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/La sociedad y la cultura/ La cultura de masas</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Los problemas y conflictos sociales</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Las transformaciones sociales</t>
+  </si>
+  <si>
+    <t>2ESO/Ciencias sociales, geografìa e historia /La organización del mundo actual/ El ser humano, un ser social/Consolidación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,13 +326,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -783,7 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -819,14 +813,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1509,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1520,7 @@
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1531,23 +1528,23 @@
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>48</v>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="21" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1555,7 +1552,7 @@
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="21">
         <v>11</v>
       </c>
     </row>
@@ -1563,7 +1560,7 @@
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="21" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1580,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1588,7 @@
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -1618,24 +1615,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -1644,171 +1641,191 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>39</v>
+      <c r="C3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="F3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>42</v>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="F4">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
+      <c r="E6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="8"/>
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="8"/>
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
+      </c>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="9"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1826,7 +1843,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:G17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1865,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>27</v>
@@ -1859,7 +1876,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
@@ -1870,7 +1887,7 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>27</v>
@@ -1881,7 +1898,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>27</v>
@@ -1934,7 +1951,7 @@
     <row r="18" spans="1:7" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="E18" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>26</v>
@@ -1949,7 +1966,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>26</v>
@@ -1961,7 +1978,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>27</v>
@@ -1974,7 +1991,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>26</v>
@@ -2002,7 +2019,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A2:C19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -2039,7 +2056,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>26</v>
@@ -2050,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -2061,7 +2078,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>26</v>
@@ -2072,7 +2089,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>26</v>
@@ -2083,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>26</v>
@@ -2094,7 +2111,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
@@ -2105,7 +2122,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
@@ -2116,7 +2133,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>26</v>
@@ -2127,7 +2144,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>26</v>
@@ -2138,7 +2155,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>26</v>
@@ -2149,7 +2166,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>26</v>
@@ -2160,7 +2177,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>27</v>
@@ -2171,7 +2188,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>26</v>
@@ -2182,7 +2199,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>26</v>
@@ -2193,7 +2210,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>26</v>
@@ -2204,7 +2221,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>27</v>
@@ -2215,22 +2232,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="18"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="18"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="18"/>
+      <c r="C25" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2249,11 +2266,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,10 +2317,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>20</v>
@@ -2316,10 +2333,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>23</v>
@@ -2332,10 +2349,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
@@ -2348,10 +2365,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>25</v>
@@ -2361,7 +2378,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>27</v>
@@ -2369,10 +2386,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>24</v>
@@ -2382,7 +2399,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>26</v>
@@ -2390,14 +2407,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>20</v>
@@ -2408,14 +2425,14 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>23</v>
@@ -2426,14 +2443,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>20</v>
@@ -2444,14 +2461,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>22</v>
@@ -2462,14 +2479,14 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>20</v>
@@ -2480,14 +2497,14 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>23</v>
@@ -2498,14 +2515,14 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>23</v>
@@ -2517,14 +2534,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>23</v>
@@ -2535,14 +2552,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>25</v>
@@ -2550,7 +2567,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>26</v>
@@ -2558,14 +2575,14 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>25</v>
@@ -2573,7 +2590,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>26</v>
@@ -2581,14 +2598,14 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>24</v>
@@ -2596,7 +2613,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>26</v>
@@ -2604,14 +2621,14 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>20</v>
@@ -2623,14 +2640,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>24</v>
@@ -2638,7 +2655,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>26</v>
@@ -2646,18 +2663,18 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>20</v>
@@ -2666,18 +2683,18 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>22</v>
@@ -2686,18 +2703,18 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>23</v>
@@ -2706,18 +2723,18 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>22</v>
@@ -2726,24 +2743,24 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>27</v>
@@ -2751,18 +2768,18 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>20</v>
@@ -2771,16 +2788,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>23</v>
@@ -2788,16 +2805,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>22</v>
@@ -2806,22 +2823,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H28" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>27</v>
@@ -2829,16 +2846,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>20</v>
@@ -2846,16 +2863,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>21</v>
@@ -2863,16 +2880,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>20</v>
@@ -2880,55 +2897,67 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>23</v>
+        <v>65</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
+        <v>51</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>20</v>
@@ -2936,243 +2965,231 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" t="s">
-        <v>68</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>20</v>
+        <v>52</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H40" s="3"/>
-      <c r="I40" s="8"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H42" t="s">
-        <v>67</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>23</v>
+      <c r="H44" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H48" t="s">
-        <v>70</v>
-      </c>
-      <c r="I48" s="5" t="s">
+      <c r="H50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>28</v>
@@ -3181,7 +3198,7 @@
         <v>29</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>26</v>
@@ -3189,33 +3206,33 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>74</v>
+        <v>29</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>75</v>
+        <v>37</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>26</v>
@@ -3223,15 +3240,49 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H54" s="2"/>
+      <c r="C54" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3249,7 +3300,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3268,7 +3319,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
@@ -3276,7 +3327,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -3284,7 +3335,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -3292,7 +3343,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -3300,7 +3351,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
@@ -3308,7 +3359,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>26</v>
@@ -3316,7 +3367,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>27</v>
@@ -3324,7 +3375,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>27</v>
@@ -3332,7 +3383,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -3340,7 +3391,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>26</v>
@@ -3348,7 +3399,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>26</v>
@@ -3356,7 +3407,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -3364,7 +3415,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>27</v>
@@ -3372,7 +3423,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>26</v>
@@ -3380,7 +3431,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
@@ -3388,7 +3439,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>26</v>
@@ -3396,7 +3447,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>27</v>
@@ -3404,7 +3455,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>26</v>

</xml_diff>